<commit_message>
Updated Excel file with sprint-by-sprint data
- Added updated sprint data
- Included story point totals
- Calculated and added average values
- Improved overall formatting for clarity
</commit_message>
<xml_diff>
--- a/User Stories/Planning Poker/user_stories.xlsx
+++ b/User Stories/Planning Poker/user_stories.xlsx
@@ -5,22 +5,35 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sanil\Projects\software year 3 group\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sanil\Projects\CO3095 YEAR 3 SOFTWARE\User Stories\Planning Poker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D124A9CF-54EA-473F-A1A2-E9D03B402F52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E95B55A4-E547-4C19-80FC-4CF0DF3D7935}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User Stories" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t>User Story</t>
   </si>
@@ -173,13 +186,25 @@
   </si>
   <si>
     <t>As a user, I want to rate songs and view the rated songs in a playlist (playlist of tracks rated 10, 9, 8, etc.) so that I have a compilation of songs that I feel similarly about.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sprint </t>
+  </si>
+  <si>
+    <t>Sprint Story Point Total</t>
+  </si>
+  <si>
+    <t>Total Story Points:</t>
+  </si>
+  <si>
+    <t>Average Story Points:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -208,6 +233,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -229,11 +269,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -536,9 +590,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C49"/>
+  <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A52" sqref="A52"/>
     </sheetView>
   </sheetViews>
@@ -547,20 +601,27 @@
     <col min="1" max="1" width="135.6640625" customWidth="1"/>
     <col min="2" max="2" width="14.5546875" customWidth="1"/>
     <col min="3" max="3" width="15.44140625" customWidth="1"/>
+    <col min="5" max="5" width="19.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="B1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -570,8 +631,11 @@
       <c r="C2">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -581,8 +645,11 @@
       <c r="C3">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -592,8 +659,11 @@
       <c r="C4">
         <v>2.25</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -603,8 +673,11 @@
       <c r="C5">
         <v>2.25</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D5" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -614,8 +687,11 @@
       <c r="C6">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D6" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -625,8 +701,15 @@
       <c r="C7">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D7" s="1">
+        <v>1</v>
+      </c>
+      <c r="E7" s="5">
+        <f>SUM(B2:B13)</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -636,8 +719,11 @@
       <c r="C8">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D8" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -647,8 +733,11 @@
       <c r="C9">
         <v>2.25</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D9" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -658,8 +747,11 @@
       <c r="C10">
         <v>0.88</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D10" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
@@ -669,8 +761,11 @@
       <c r="C11">
         <v>1.1299999999999999</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D11" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>43</v>
       </c>
@@ -680,8 +775,11 @@
       <c r="C12">
         <v>3.5</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D12" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>37</v>
       </c>
@@ -691,8 +789,11 @@
       <c r="C13">
         <v>5</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D13" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
@@ -702,8 +803,11 @@
       <c r="C14">
         <v>2.75</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D14" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
@@ -713,8 +817,11 @@
       <c r="C15">
         <v>3.5</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D15" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
@@ -724,8 +831,11 @@
       <c r="C16">
         <v>3.5</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D16" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>16</v>
       </c>
@@ -735,8 +845,11 @@
       <c r="C17">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D17" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>17</v>
       </c>
@@ -746,8 +859,11 @@
       <c r="C18">
         <v>2.75</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D18" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>18</v>
       </c>
@@ -757,8 +873,15 @@
       <c r="C19">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D19" s="2">
+        <v>2</v>
+      </c>
+      <c r="E19" s="6">
+        <f>SUM(B14:B25)</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>19</v>
       </c>
@@ -768,8 +891,11 @@
       <c r="C20">
         <v>2.75</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D20" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>20</v>
       </c>
@@ -779,8 +905,11 @@
       <c r="C21">
         <v>0.88</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D21" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>21</v>
       </c>
@@ -790,8 +919,11 @@
       <c r="C22">
         <v>5.75</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D22" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>22</v>
       </c>
@@ -801,8 +933,11 @@
       <c r="C23">
         <v>1.75</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D23" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>23</v>
       </c>
@@ -812,8 +947,11 @@
       <c r="C24">
         <v>5.75</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D24" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>24</v>
       </c>
@@ -823,8 +961,11 @@
       <c r="C25">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D25" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>25</v>
       </c>
@@ -834,8 +975,11 @@
       <c r="C26">
         <v>6.5</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D26" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>26</v>
       </c>
@@ -845,8 +989,11 @@
       <c r="C27">
         <v>4</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D27" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>27</v>
       </c>
@@ -856,8 +1003,11 @@
       <c r="C28">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D28" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>28</v>
       </c>
@@ -867,8 +1017,11 @@
       <c r="C29">
         <v>5.75</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D29" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>29</v>
       </c>
@@ -878,8 +1031,11 @@
       <c r="C30">
         <v>4</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D30" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>30</v>
       </c>
@@ -889,8 +1045,15 @@
       <c r="C31">
         <v>1.75</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D31" s="3">
+        <v>3</v>
+      </c>
+      <c r="E31" s="4">
+        <f>SUM(B26:B37)</f>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>31</v>
       </c>
@@ -900,8 +1063,11 @@
       <c r="C32">
         <v>6.5</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D32" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
         <v>32</v>
       </c>
@@ -911,8 +1077,11 @@
       <c r="C33">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D33" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
         <v>33</v>
       </c>
@@ -922,8 +1091,11 @@
       <c r="C34">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D34" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>34</v>
       </c>
@@ -933,8 +1105,11 @@
       <c r="C35">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D35" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>35</v>
       </c>
@@ -944,8 +1119,11 @@
       <c r="C36">
         <v>2.75</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D36" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
         <v>36</v>
       </c>
@@ -955,9 +1133,12 @@
       <c r="C37">
         <v>2.75</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
+      <c r="D37" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" s="7" t="s">
         <v>12</v>
       </c>
       <c r="B38">
@@ -966,9 +1147,12 @@
       <c r="C38">
         <v>6.5</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
+      <c r="D38" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" s="7" t="s">
         <v>38</v>
       </c>
       <c r="B39">
@@ -977,9 +1161,12 @@
       <c r="C39">
         <v>5</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
+      <c r="D39" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" s="7" t="s">
         <v>39</v>
       </c>
       <c r="B40">
@@ -988,9 +1175,12 @@
       <c r="C40">
         <v>6.5</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
+      <c r="D40" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" s="7" t="s">
         <v>40</v>
       </c>
       <c r="B41">
@@ -999,9 +1189,12 @@
       <c r="C41">
         <v>4</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A42" s="2" t="s">
+      <c r="D41" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" s="7" t="s">
         <v>41</v>
       </c>
       <c r="B42">
@@ -1010,9 +1203,12 @@
       <c r="C42">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A43" s="2" t="s">
+      <c r="D42" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" s="7" t="s">
         <v>42</v>
       </c>
       <c r="B43">
@@ -1021,9 +1217,16 @@
       <c r="C43">
         <v>3</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A44" s="2" t="s">
+      <c r="D43" s="7">
+        <v>4</v>
+      </c>
+      <c r="E43" s="8">
+        <f>SUM(B38:B49)</f>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" s="7" t="s">
         <v>45</v>
       </c>
       <c r="B44">
@@ -1032,9 +1235,12 @@
       <c r="C44">
         <v>5.75</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
+      <c r="D44" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" s="7" t="s">
         <v>46</v>
       </c>
       <c r="B45">
@@ -1043,9 +1249,12 @@
       <c r="C45">
         <v>5</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
+      <c r="D45" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" s="7" t="s">
         <v>47</v>
       </c>
       <c r="B46">
@@ -1054,9 +1263,12 @@
       <c r="C46">
         <v>6.5</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A47" s="2" t="s">
+      <c r="D46" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" s="7" t="s">
         <v>48</v>
       </c>
       <c r="B47">
@@ -1065,9 +1277,12 @@
       <c r="C47">
         <v>3.5</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A48" s="2" t="s">
+      <c r="D47" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48" s="7" t="s">
         <v>49</v>
       </c>
       <c r="B48">
@@ -1076,9 +1291,12 @@
       <c r="C48">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A49" s="2" t="s">
+      <c r="D48" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" s="7" t="s">
         <v>50</v>
       </c>
       <c r="B49">
@@ -1087,6 +1305,38 @@
       <c r="C49">
         <v>4</v>
       </c>
+      <c r="D49" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B50">
+        <f>SUM(B2:B49)</f>
+        <v>203</v>
+      </c>
+      <c r="C50">
+        <f>SUM(C2:C49)</f>
+        <v>175.39</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B51">
+        <f>AVERAGE(B2:B49)</f>
+        <v>4.229166666666667</v>
+      </c>
+      <c r="C51">
+        <f>AVERAGE(C2:C49)</f>
+        <v>3.6539583333333332</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Added Time Estimates to user_stories.xlsx
</commit_message>
<xml_diff>
--- a/User Stories/Planning Poker/user_stories.xlsx
+++ b/User Stories/Planning Poker/user_stories.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sanil\Projects\CO3095 YEAR 3 SOFTWARE\User Stories\Planning Poker\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raygu\Downloads\CO3095-Group-16-Music-Player-Application\User Stories\Planning Poker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E95B55A4-E547-4C19-80FC-4CF0DF3D7935}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40FEF03F-426D-46A0-B324-91FCE2E297B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User Stories" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <si>
     <t>User Story</t>
   </si>
@@ -198,6 +198,15 @@
   </si>
   <si>
     <t>Average Story Points:</t>
+  </si>
+  <si>
+    <t>Optimistic (Hours)</t>
+  </si>
+  <si>
+    <t>Most Likely (Hours)</t>
+  </si>
+  <si>
+    <t>Pessimistic (Hours)</t>
   </si>
 </sst>
 </file>
@@ -590,21 +599,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E53"/>
+  <dimension ref="A1:H53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="135.6640625" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" customWidth="1"/>
-    <col min="3" max="3" width="15.44140625" customWidth="1"/>
-    <col min="5" max="5" width="19.109375" customWidth="1"/>
+    <col min="1" max="1" width="135.7109375" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" customWidth="1"/>
+    <col min="5" max="5" width="21.7109375" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" customWidth="1"/>
+    <col min="7" max="7" width="18.7109375" customWidth="1"/>
+    <col min="8" max="8" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -620,8 +632,17 @@
       <c r="E1" s="9" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -634,8 +655,19 @@
       <c r="D2" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F2">
+        <f>(B2*0.5)</f>
+        <v>2.5</v>
+      </c>
+      <c r="G2">
+        <v>5</v>
+      </c>
+      <c r="H2">
+        <f>(B2*1.5)</f>
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -648,8 +680,19 @@
       <c r="D3" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F3">
+        <f t="shared" ref="F3:F49" si="0">(B3*0.5)</f>
+        <v>2.5</v>
+      </c>
+      <c r="G3">
+        <v>5</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H49" si="1">(B3*1.5)</f>
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -662,8 +705,19 @@
       <c r="D4" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>2</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -676,8 +730,19 @@
       <c r="D5" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>2</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -690,8 +755,19 @@
       <c r="D6" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+      <c r="G6">
+        <v>3</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="1"/>
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -708,8 +784,19 @@
         <f>SUM(B2:B13)</f>
         <v>35</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+      <c r="G7">
+        <v>3</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="1"/>
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -722,8 +809,19 @@
       <c r="D8" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+      <c r="G8">
+        <v>3</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="1"/>
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -736,8 +834,19 @@
       <c r="D9" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>2</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -750,8 +859,19 @@
       <c r="D10" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="1"/>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
@@ -764,8 +884,19 @@
       <c r="D11" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="1"/>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>43</v>
       </c>
@@ -778,8 +909,19 @@
       <c r="D12" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+      <c r="G12">
+        <v>3</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="1"/>
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>37</v>
       </c>
@@ -792,8 +934,19 @@
       <c r="D13" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="G13">
+        <v>5</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="1"/>
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
@@ -806,8 +959,19 @@
       <c r="D14" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+      <c r="G14">
+        <v>3</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="1"/>
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
@@ -820,8 +984,19 @@
       <c r="D15" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="G15">
+        <v>5</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="1"/>
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
@@ -834,8 +1009,19 @@
       <c r="D16" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F16">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="G16">
+        <v>5</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="1"/>
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>16</v>
       </c>
@@ -848,8 +1034,19 @@
       <c r="D17" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F17">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>2</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>17</v>
       </c>
@@ -862,8 +1059,19 @@
       <c r="D18" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F18">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+      <c r="G18">
+        <v>3</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="1"/>
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>18</v>
       </c>
@@ -880,8 +1088,19 @@
         <f>SUM(B14:B25)</f>
         <v>40</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F19">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+      <c r="G19">
+        <v>3</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="1"/>
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>19</v>
       </c>
@@ -894,8 +1113,19 @@
       <c r="D20" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F20">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+      <c r="G20">
+        <v>3</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="1"/>
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>20</v>
       </c>
@@ -908,8 +1138,19 @@
       <c r="D21" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F21">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="1"/>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>21</v>
       </c>
@@ -922,8 +1163,19 @@
       <c r="D22" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F22">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="G22">
+        <v>5</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="1"/>
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>22</v>
       </c>
@@ -936,8 +1188,19 @@
       <c r="D23" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F23">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <v>2</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>23</v>
       </c>
@@ -950,8 +1213,19 @@
       <c r="D24" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F24">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="G24">
+        <v>5</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="1"/>
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>24</v>
       </c>
@@ -964,8 +1238,19 @@
       <c r="D25" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F25">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+      <c r="G25">
+        <v>3</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="1"/>
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>25</v>
       </c>
@@ -978,8 +1263,19 @@
       <c r="D26" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F26">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="G26">
+        <v>8</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>26</v>
       </c>
@@ -992,8 +1288,19 @@
       <c r="D27" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F27">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="G27">
+        <v>5</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="1"/>
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>27</v>
       </c>
@@ -1006,8 +1313,19 @@
       <c r="D28" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F28">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="G28">
+        <v>5</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="1"/>
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>28</v>
       </c>
@@ -1020,8 +1338,19 @@
       <c r="D29" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F29">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="G29">
+        <v>8</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>29</v>
       </c>
@@ -1034,8 +1363,19 @@
       <c r="D30" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F30">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="G30">
+        <v>5</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="1"/>
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>30</v>
       </c>
@@ -1052,8 +1392,19 @@
         <f>SUM(B26:B37)</f>
         <v>58</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F31">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G31">
+        <v>2</v>
+      </c>
+      <c r="H31">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>31</v>
       </c>
@@ -1066,8 +1417,19 @@
       <c r="D32" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F32">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="G32">
+        <v>8</v>
+      </c>
+      <c r="H32">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>32</v>
       </c>
@@ -1080,8 +1442,19 @@
       <c r="D33" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F33">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+      <c r="G33">
+        <v>3</v>
+      </c>
+      <c r="H33">
+        <f t="shared" si="1"/>
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>33</v>
       </c>
@@ -1094,8 +1467,19 @@
       <c r="D34" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F34">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+      <c r="G34">
+        <v>3</v>
+      </c>
+      <c r="H34">
+        <f t="shared" si="1"/>
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>34</v>
       </c>
@@ -1108,8 +1492,19 @@
       <c r="D35" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F35">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="G35">
+        <v>5</v>
+      </c>
+      <c r="H35">
+        <f t="shared" si="1"/>
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>35</v>
       </c>
@@ -1122,8 +1517,19 @@
       <c r="D36" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F36">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+      <c r="G36">
+        <v>3</v>
+      </c>
+      <c r="H36">
+        <f t="shared" si="1"/>
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>36</v>
       </c>
@@ -1136,8 +1542,19 @@
       <c r="D37" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F37">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+      <c r="G37">
+        <v>3</v>
+      </c>
+      <c r="H37">
+        <f t="shared" si="1"/>
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
         <v>12</v>
       </c>
@@ -1150,8 +1567,19 @@
       <c r="D38" s="7">
         <v>4</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F38">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="G38">
+        <v>8</v>
+      </c>
+      <c r="H38">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
         <v>38</v>
       </c>
@@ -1164,8 +1592,19 @@
       <c r="D39" s="7">
         <v>4</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F39">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="G39">
+        <v>5</v>
+      </c>
+      <c r="H39">
+        <f t="shared" si="1"/>
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
         <v>39</v>
       </c>
@@ -1178,8 +1617,19 @@
       <c r="D40" s="7">
         <v>4</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F40">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="G40">
+        <v>8</v>
+      </c>
+      <c r="H40">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
         <v>40</v>
       </c>
@@ -1192,8 +1642,19 @@
       <c r="D41" s="7">
         <v>4</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F41">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="G41">
+        <v>5</v>
+      </c>
+      <c r="H41">
+        <f t="shared" si="1"/>
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
         <v>41</v>
       </c>
@@ -1206,8 +1667,19 @@
       <c r="D42" s="7">
         <v>4</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F42">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="G42">
+        <v>5</v>
+      </c>
+      <c r="H42">
+        <f t="shared" si="1"/>
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
         <v>42</v>
       </c>
@@ -1224,8 +1696,19 @@
         <f>SUM(B38:B49)</f>
         <v>70</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F43">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+      <c r="G43">
+        <v>3</v>
+      </c>
+      <c r="H43">
+        <f t="shared" si="1"/>
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
         <v>45</v>
       </c>
@@ -1238,8 +1721,19 @@
       <c r="D44" s="7">
         <v>4</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F44">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="G44">
+        <v>8</v>
+      </c>
+      <c r="H44">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
         <v>46</v>
       </c>
@@ -1252,8 +1746,19 @@
       <c r="D45" s="7">
         <v>4</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F45">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="G45">
+        <v>5</v>
+      </c>
+      <c r="H45">
+        <f t="shared" si="1"/>
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
         <v>47</v>
       </c>
@@ -1266,8 +1771,19 @@
       <c r="D46" s="7">
         <v>4</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F46">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="G46">
+        <v>8</v>
+      </c>
+      <c r="H46">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
         <v>48</v>
       </c>
@@ -1280,8 +1796,19 @@
       <c r="D47" s="7">
         <v>4</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F47">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="G47">
+        <v>5</v>
+      </c>
+      <c r="H47">
+        <f t="shared" si="1"/>
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
         <v>49</v>
       </c>
@@ -1294,8 +1821,19 @@
       <c r="D48" s="7">
         <v>4</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F48">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="G48">
+        <v>5</v>
+      </c>
+      <c r="H48">
+        <f t="shared" si="1"/>
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
         <v>50</v>
       </c>
@@ -1308,8 +1846,19 @@
       <c r="D49" s="7">
         <v>4</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F49">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="G49">
+        <v>5</v>
+      </c>
+      <c r="H49">
+        <f t="shared" si="1"/>
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="9" t="s">
         <v>53</v>
       </c>
@@ -1322,7 +1871,7 @@
         <v>175.39</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="9" t="s">
         <v>54</v>
       </c>
@@ -1335,7 +1884,7 @@
         <v>3.6539583333333332</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Expected Time to user_stories.xlsx
</commit_message>
<xml_diff>
--- a/User Stories/Planning Poker/user_stories.xlsx
+++ b/User Stories/Planning Poker/user_stories.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raygu\Downloads\CO3095-Group-16-Music-Player-Application\User Stories\Planning Poker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40FEF03F-426D-46A0-B324-91FCE2E297B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B4221FB-5F3D-44D2-BF04-BCDCFA2AE40C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
   <si>
     <t>User Story</t>
   </si>
@@ -207,6 +207,9 @@
   </si>
   <si>
     <t>Pessimistic (Hours)</t>
+  </si>
+  <si>
+    <t>Expected (Hours)</t>
   </si>
 </sst>
 </file>
@@ -599,7 +602,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H53"/>
+  <dimension ref="A1:I53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I1" sqref="I1"/>
@@ -614,9 +617,10 @@
     <col min="6" max="6" width="17.42578125" customWidth="1"/>
     <col min="7" max="7" width="18.7109375" customWidth="1"/>
     <col min="8" max="8" width="17.85546875" customWidth="1"/>
+    <col min="9" max="9" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -641,8 +645,11 @@
       <c r="H1" s="9" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" s="9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -666,8 +673,12 @@
         <f>(B2*1.5)</f>
         <v>7.5</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2">
+        <f>((F2+(4*G2)+H2)/6)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -691,8 +702,12 @@
         <f t="shared" ref="H3:H49" si="1">(B3*1.5)</f>
         <v>7.5</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3">
+        <f t="shared" ref="I3:I49" si="2">((F3+(4*G3)+H3)/6)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -716,8 +731,12 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -741,8 +760,12 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -766,8 +789,12 @@
         <f t="shared" si="1"/>
         <v>4.5</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -795,8 +822,12 @@
         <f t="shared" si="1"/>
         <v>4.5</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I7">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -820,8 +851,12 @@
         <f t="shared" si="1"/>
         <v>4.5</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -845,8 +880,12 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I9">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -870,8 +909,12 @@
         <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
@@ -895,8 +938,12 @@
         <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I11">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>43</v>
       </c>
@@ -920,8 +967,12 @@
         <f t="shared" si="1"/>
         <v>4.5</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I12">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>37</v>
       </c>
@@ -945,8 +996,12 @@
         <f t="shared" si="1"/>
         <v>7.5</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I13">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
@@ -970,8 +1025,12 @@
         <f t="shared" si="1"/>
         <v>4.5</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I14">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
@@ -995,8 +1054,12 @@
         <f t="shared" si="1"/>
         <v>7.5</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I15">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
@@ -1020,8 +1083,12 @@
         <f t="shared" si="1"/>
         <v>7.5</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I16">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>16</v>
       </c>
@@ -1045,8 +1112,12 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I17">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>17</v>
       </c>
@@ -1070,8 +1141,12 @@
         <f t="shared" si="1"/>
         <v>4.5</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I18">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>18</v>
       </c>
@@ -1099,8 +1174,12 @@
         <f t="shared" si="1"/>
         <v>4.5</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I19">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>19</v>
       </c>
@@ -1124,8 +1203,12 @@
         <f t="shared" si="1"/>
         <v>4.5</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I20">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>20</v>
       </c>
@@ -1149,8 +1232,12 @@
         <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I21">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>21</v>
       </c>
@@ -1174,8 +1261,12 @@
         <f t="shared" si="1"/>
         <v>7.5</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I22">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>22</v>
       </c>
@@ -1199,8 +1290,12 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I23">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>23</v>
       </c>
@@ -1224,8 +1319,12 @@
         <f t="shared" si="1"/>
         <v>7.5</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I24">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>24</v>
       </c>
@@ -1249,8 +1348,12 @@
         <f t="shared" si="1"/>
         <v>4.5</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I25">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>25</v>
       </c>
@@ -1274,8 +1377,12 @@
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I26">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>26</v>
       </c>
@@ -1299,8 +1406,12 @@
         <f t="shared" si="1"/>
         <v>7.5</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I27">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>27</v>
       </c>
@@ -1324,8 +1435,12 @@
         <f t="shared" si="1"/>
         <v>7.5</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I28">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>28</v>
       </c>
@@ -1349,8 +1464,12 @@
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I29">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>29</v>
       </c>
@@ -1374,8 +1493,12 @@
         <f t="shared" si="1"/>
         <v>7.5</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I30">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>30</v>
       </c>
@@ -1403,8 +1526,12 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I31">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>31</v>
       </c>
@@ -1428,8 +1555,12 @@
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I32">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>32</v>
       </c>
@@ -1453,8 +1584,12 @@
         <f t="shared" si="1"/>
         <v>4.5</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I33">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>33</v>
       </c>
@@ -1478,8 +1613,12 @@
         <f t="shared" si="1"/>
         <v>4.5</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I34">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>34</v>
       </c>
@@ -1503,8 +1642,12 @@
         <f t="shared" si="1"/>
         <v>7.5</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I35">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>35</v>
       </c>
@@ -1528,8 +1671,12 @@
         <f t="shared" si="1"/>
         <v>4.5</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I36">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>36</v>
       </c>
@@ -1553,8 +1700,12 @@
         <f t="shared" si="1"/>
         <v>4.5</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I37">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
         <v>12</v>
       </c>
@@ -1578,8 +1729,12 @@
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I38">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
         <v>38</v>
       </c>
@@ -1603,8 +1758,12 @@
         <f t="shared" si="1"/>
         <v>7.5</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I39">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
         <v>39</v>
       </c>
@@ -1628,8 +1787,12 @@
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I40">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
         <v>40</v>
       </c>
@@ -1653,8 +1816,12 @@
         <f t="shared" si="1"/>
         <v>7.5</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I41">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
         <v>41</v>
       </c>
@@ -1678,8 +1845,12 @@
         <f t="shared" si="1"/>
         <v>7.5</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I42">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
         <v>42</v>
       </c>
@@ -1707,8 +1878,12 @@
         <f t="shared" si="1"/>
         <v>4.5</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I43">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
         <v>45</v>
       </c>
@@ -1732,8 +1907,12 @@
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I44">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
         <v>46</v>
       </c>
@@ -1757,8 +1936,12 @@
         <f t="shared" si="1"/>
         <v>7.5</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I45">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
         <v>47</v>
       </c>
@@ -1782,8 +1965,12 @@
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I46">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
         <v>48</v>
       </c>
@@ -1807,8 +1994,12 @@
         <f t="shared" si="1"/>
         <v>7.5</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I47">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
         <v>49</v>
       </c>
@@ -1832,8 +2023,12 @@
         <f t="shared" si="1"/>
         <v>7.5</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I48">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
         <v>50</v>
       </c>
@@ -1857,8 +2052,12 @@
         <f t="shared" si="1"/>
         <v>7.5</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I49">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="9" t="s">
         <v>53</v>
       </c>
@@ -1871,7 +2070,7 @@
         <v>175.39</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="9" t="s">
         <v>54</v>
       </c>
@@ -1884,7 +2083,7 @@
         <v>3.6539583333333332</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
     </row>
   </sheetData>

</xml_diff>